<commit_message>
Working on Gson json object format. Not working version
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16020" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>post</t>
   </si>
@@ -24,10 +24,7 @@
     <t>https://jsonplaceholder.typicode.com/posts</t>
   </si>
   <si>
-    <t>{\"title\": \"jonnyalexfoo1\", \"body\": \"bar\", \"userId\": 5 }</t>
-  </si>
-  <si>
-    <t>{\"title\": \"jonnyalexfoo2\", \"body\": \"bar\", \"userId\": 5 }</t>
+    <t>{\"title\": \"jonnyalexfoo1\", \"body\": \"bar\", \"userId\": \"5\"}</t>
   </si>
 </sst>
 </file>
@@ -372,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -382,7 +379,7 @@
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -396,17 +393,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>

</xml_diff>

<commit_message>
Added comments to code, and implemented PUT and DELETE
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>post</t>
   </si>
@@ -25,6 +25,27 @@
   </si>
   <si>
     <t>{"title": "jonnyalexfoo1", "body": "bar", "userId": "5"}</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>https://jsonplaceholder.typicode.com/posts/1</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>{"title": "jonnyalexfoo1", "body": "bar", "userId": "1"}</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>{"title": "null", "body": "null", "userId": "1"}</t>
   </si>
 </sst>
 </file>
@@ -369,33 +390,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
     <col min="3" max="3" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>